<commit_message>
minor revisions to seagrass data entry spreadsheets
</commit_message>
<xml_diff>
--- a/seagrass/final_spreadsheets/marinegeo_spreadsheet_seagrass_shoots.xlsx
+++ b/seagrass/final_spreadsheets/marinegeo_spreadsheet_seagrass_shoots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\spreadsheets_final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\seagrass\final_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B799C19B-C7CC-40F0-8977-B0E048BE9BC3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A13DDE-9D3B-4588-8ED8-A4B86E0B4E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="2040" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="114">
   <si>
     <t>sheet</t>
   </si>
@@ -1772,7 +1772,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2195,9 +2195,7 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -2580,7 +2578,7 @@
   <sheetPr>
     <tabColor rgb="FF97C8EB"/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2884,16 +2882,16 @@
         <v>63</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -2902,16 +2900,16 @@
         <v>63</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F19" s="5"/>
     </row>
@@ -2920,25 +2918,25 @@
         <v>63</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" s="23" customFormat="1" ht="56.1" customHeight="1">
+    <row r="21" spans="1:6" s="19" customFormat="1" ht="56.1" customHeight="1">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>34</v>
@@ -2947,25 +2945,25 @@
         <v>30</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" s="19" customFormat="1" ht="56.1" customHeight="1">
+    <row r="22" spans="1:6" s="23" customFormat="1" ht="56.1" customHeight="1">
       <c r="A22" s="5" t="s">
         <v>63</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F22" s="5"/>
     </row>
@@ -3399,15 +3397,15 @@
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" spans="1:6" s="23" customFormat="1" ht="51" customHeight="1">
+    <row r="49" spans="1:6" s="23" customFormat="1" ht="49.5" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>39</v>
@@ -3419,15 +3417,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="23" customFormat="1" ht="54.75" customHeight="1">
+    <row r="50" spans="1:6" s="23" customFormat="1" ht="60" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>39</v>
@@ -3435,57 +3433,57 @@
       <c r="E50" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" s="23" customFormat="1" ht="49.5" customHeight="1">
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" s="23" customFormat="1" ht="57.75" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" s="23" customFormat="1" ht="60" customHeight="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="20" customFormat="1" ht="66" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F52" s="4"/>
-    </row>
-    <row r="53" spans="1:6" s="23" customFormat="1" ht="57.75" customHeight="1">
+        <v>38</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="20" customFormat="1" ht="69.75" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>39</v>
@@ -3497,15 +3495,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="20" customFormat="1" ht="66" customHeight="1">
+    <row r="54" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>39</v>
@@ -3517,99 +3515,91 @@
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="20" customFormat="1" ht="69.75" customHeight="1">
+    <row r="55" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
       <c r="A55" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="40" t="s">
-        <v>82</v>
+      <c r="B55" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A56" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B56" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F56" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
-      <c r="A57" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D57" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A56" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="15"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="15"/>
+    </row>
+    <row r="57" spans="1:6" ht="50.1" customHeight="1">
+      <c r="A57" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" s="9"/>
+      <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="15"/>
+      <c r="B58" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="1:6" ht="50.1" customHeight="1">
       <c r="A59" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E59" s="9"/>
-      <c r="F59" s="5"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="1:6" ht="50.1" customHeight="1">
       <c r="A60" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>17</v>
@@ -3622,64 +3612,32 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" ht="50.1" customHeight="1">
       <c r="A62" s="5" t="s">
         <v>58</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
-    </row>
-    <row r="63" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A63" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E63" s="9"/>
-      <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:6" ht="50.1" customHeight="1">
-      <c r="A64" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4:B5 B9:B12">
@@ -3703,7 +3661,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B19:B22" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Latitude in decimal degrees to five decimal places" sqref="B18:B22" xr:uid="{00000000-0002-0000-0400-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The units the field should contain" sqref="F1" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The format the field should follow" sqref="E1" xr:uid="{00000000-0002-0000-0400-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The type of entry that should occupy the field (e.g., text, decimal, integer, date, etc…)" sqref="D1" xr:uid="{00000000-0002-0000-0400-000003000000}"/>

</xml_diff>

<commit_message>
update seagrass shoots data entry spreadsheet
</commit_message>
<xml_diff>
--- a/seagrass/final_spreadsheets/marinegeo_spreadsheet_seagrass_shoots.xlsx
+++ b/seagrass/final_spreadsheets/marinegeo_spreadsheet_seagrass_shoots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlonn\Documents\Repositories\protocols\seagrass\final_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A13DDE-9D3B-4588-8ED8-A4B86E0B4E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CA0387-DDE2-4416-BF2A-E79704D99C31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="protocol_metadata" sheetId="1" r:id="rId1"/>
@@ -315,12 +315,6 @@
     <t>site_code</t>
   </si>
   <si>
-    <t>number_grazing_scars</t>
-  </si>
-  <si>
-    <t>Number of grazing scars on seagrass blades</t>
-  </si>
-  <si>
     <t>data_entry_day</t>
   </si>
   <si>
@@ -417,6 +411,12 @@
   </si>
   <si>
     <t>v0.5.0</t>
+  </si>
+  <si>
+    <t>grazing_scars_present</t>
+  </si>
+  <si>
+    <t>Indicate whether grazing scars were present, 1 = grazing scars present; 0 = no grazing scars present</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1246,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1258,7 +1258,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="161.1" customHeight="1">
       <c r="B1" s="39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1283,19 +1283,19 @@
     </row>
     <row r="5" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B6" s="11"/>
     </row>
     <row r="7" spans="1:2" ht="39.950000000000003" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B7" s="11"/>
     </row>
@@ -1316,7 +1316,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="39.950000000000003" customHeight="1">
@@ -1442,13 +1442,13 @@
         <v>74</v>
       </c>
       <c r="K1" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L1" s="29" t="s">
         <v>52</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1805,16 +1805,16 @@
         <v>75</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J1" s="32" t="s">
         <v>76</v>
@@ -1823,7 +1823,7 @@
         <v>77</v>
       </c>
       <c r="L1" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -2195,7 +2195,7 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -2229,19 +2229,19 @@
         <v>75</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H1" s="29" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="32" t="s">
         <v>78</v>
       </c>
       <c r="J1" s="32" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="K1" s="32" t="s">
         <v>79</v>
@@ -2256,7 +2256,7 @@
         <v>81</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -2554,7 +2554,7 @@
       <c r="H50" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="13">
+  <dataValidations count="14">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The distance along the transect that the sample was collected (from 1-50 m)" sqref="E1" xr:uid="{26323778-50F7-45F3-A0A3-19676717E5E7}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="The full name of the person processing the sample (no initials; ONLY one name per sample)" sqref="H1" xr:uid="{67ACE702-B89D-4456-BCE8-82AFE5D5D8C3}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Scientific name using standard scientific nomenclature. If the species cannot be identified to species, report genus or higher." sqref="F1" xr:uid="{B2C2B7EA-50DC-4562-BF5B-AB6CBD62C0C1}"/>
@@ -2567,7 +2567,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mass of the empty tin to hold the blades, in grams" sqref="M1" xr:uid="{FE070361-E221-42E1-BF00-56C75D61FC7E}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mass of the empty tin and epibionts that have been dried to a constant weight, in grams" sqref="L1" xr:uid="{D04A55A3-26EF-4DEA-AC36-EFE1B8B08461}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Mass of the empty tin to hold the epibionts, in grams" sqref="K1" xr:uid="{BACED461-2ABE-4483-A3F3-8AF2C4E6FA21}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sheath length in millimeters" sqref="I1:J1" xr:uid="{9BDD3B1D-7D64-4A89-8F9D-F8B1052F9BEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sheath length in millimeters" sqref="I1" xr:uid="{9BDD3B1D-7D64-4A89-8F9D-F8B1052F9BEE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Indicate whether grazing scars were present, 1 = grazing scars present; 0 = no grazing scars present" sqref="J1" xr:uid="{2C6B2DF7-D42A-4D19-9B2B-5524E510C3FC}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2581,8 +2582,8 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="50.1" customHeight="1"/>
@@ -2680,16 +2681,16 @@
         <v>64</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -2698,16 +2699,16 @@
         <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F7" s="4"/>
     </row>
@@ -2716,16 +2717,16 @@
         <v>64</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F8" s="4"/>
     </row>
@@ -2990,10 +2991,10 @@
         <v>63</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>17</v>
@@ -3009,7 +3010,7 @@
         <v>52</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>17</v>
@@ -3022,10 +3023,10 @@
         <v>63</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>17</v>
@@ -3035,7 +3036,7 @@
     </row>
     <row r="27" spans="1:6" s="23" customFormat="1" ht="31.5">
       <c r="A27" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B27" s="18"/>
       <c r="C27" s="15" t="s">
@@ -3047,7 +3048,7 @@
     </row>
     <row r="28" spans="1:6" s="23" customFormat="1" ht="45.75" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>67</v>
@@ -3065,7 +3066,7 @@
     </row>
     <row r="29" spans="1:6" s="23" customFormat="1" ht="78" customHeight="1">
       <c r="A29" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>84</v>
@@ -3083,7 +3084,7 @@
     </row>
     <row r="30" spans="1:6" s="23" customFormat="1" ht="45" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>66</v>
@@ -3099,7 +3100,7 @@
     </row>
     <row r="31" spans="1:6" s="23" customFormat="1" ht="51" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>68</v>
@@ -3115,7 +3116,7 @@
     </row>
     <row r="32" spans="1:6" s="23" customFormat="1" ht="42.75" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>75</v>
@@ -3133,13 +3134,13 @@
     </row>
     <row r="33" spans="1:6" s="36" customFormat="1" ht="66" customHeight="1">
       <c r="A33" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B33" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" s="35" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" s="35" t="s">
-        <v>100</v>
       </c>
       <c r="D33" s="35" t="s">
         <v>17</v>
@@ -3149,13 +3150,13 @@
     </row>
     <row r="34" spans="1:6" s="36" customFormat="1" ht="66" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B34" s="34" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C34" s="35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D34" s="35" t="s">
         <v>17</v>
@@ -3165,13 +3166,13 @@
     </row>
     <row r="35" spans="1:6" s="38" customFormat="1" ht="47.25">
       <c r="A35" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" s="37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" s="37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D35" s="37" t="s">
         <v>17</v>
@@ -3181,13 +3182,13 @@
     </row>
     <row r="36" spans="1:6" s="38" customFormat="1" ht="54" customHeight="1">
       <c r="A36" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C36" s="37" t="s">
         <v>108</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="37" t="s">
-        <v>110</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>30</v>
@@ -3197,7 +3198,7 @@
     </row>
     <row r="37" spans="1:6" s="23" customFormat="1" ht="51" customHeight="1">
       <c r="A37" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>76</v>
@@ -3217,7 +3218,7 @@
     </row>
     <row r="38" spans="1:6" s="23" customFormat="1" ht="54.75" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>77</v>
@@ -3237,13 +3238,13 @@
     </row>
     <row r="39" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
       <c r="A39" s="12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C39" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D39" s="24" t="s">
         <v>17</v>
@@ -3253,7 +3254,7 @@
     </row>
     <row r="40" spans="1:6" s="23" customFormat="1" ht="31.5">
       <c r="A40" s="15" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="15" t="s">
@@ -3265,7 +3266,7 @@
     </row>
     <row r="41" spans="1:6" s="23" customFormat="1" ht="45.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B41" s="40" t="s">
         <v>67</v>
@@ -3283,7 +3284,7 @@
     </row>
     <row r="42" spans="1:6" s="23" customFormat="1" ht="78" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B42" s="40" t="s">
         <v>84</v>
@@ -3301,7 +3302,7 @@
     </row>
     <row r="43" spans="1:6" s="23" customFormat="1" ht="45" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B43" s="40" t="s">
         <v>66</v>
@@ -3317,7 +3318,7 @@
     </row>
     <row r="44" spans="1:6" s="23" customFormat="1" ht="51" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B44" s="40" t="s">
         <v>68</v>
@@ -3333,7 +3334,7 @@
     </row>
     <row r="45" spans="1:6" s="23" customFormat="1" ht="42.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B45" s="40" t="s">
         <v>75</v>
@@ -3351,13 +3352,13 @@
     </row>
     <row r="46" spans="1:6" s="36" customFormat="1" ht="66" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B46" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>17</v>
@@ -3367,13 +3368,13 @@
     </row>
     <row r="47" spans="1:6" s="36" customFormat="1" ht="66" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>17</v>
@@ -3383,13 +3384,13 @@
     </row>
     <row r="48" spans="1:6" s="38" customFormat="1" ht="47.25">
       <c r="A48" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>17</v>
@@ -3399,7 +3400,7 @@
     </row>
     <row r="49" spans="1:6" s="23" customFormat="1" ht="49.5" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B49" s="40" t="s">
         <v>78</v>
@@ -3419,13 +3420,13 @@
     </row>
     <row r="50" spans="1:6" s="23" customFormat="1" ht="60" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>39</v>
@@ -3437,7 +3438,7 @@
     </row>
     <row r="51" spans="1:6" s="23" customFormat="1" ht="57.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" s="40" t="s">
         <v>79</v>
@@ -3457,7 +3458,7 @@
     </row>
     <row r="52" spans="1:6" s="20" customFormat="1" ht="66" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B52" s="40" t="s">
         <v>80</v>
@@ -3477,7 +3478,7 @@
     </row>
     <row r="53" spans="1:6" s="20" customFormat="1" ht="69.75" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B53" s="40" t="s">
         <v>82</v>
@@ -3497,7 +3498,7 @@
     </row>
     <row r="54" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" s="40" t="s">
         <v>81</v>
@@ -3517,13 +3518,13 @@
     </row>
     <row r="55" spans="1:6" s="17" customFormat="1" ht="50.1" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>17</v>

</xml_diff>